<commit_message>
Added a preliminary version of the Hale which needs to corrected for the winglet geometry
</commit_message>
<xml_diff>
--- a/aeroelasticPMOR_Optimization/design_of_experiments/prelim_results.xlsx
+++ b/aeroelasticPMOR_Optimization/design_of_experiments/prelim_results.xlsx
@@ -1,40 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://imperiallondon-my.sharepoint.com/personal/pd5118_ic_ac_uk/Documents/FYP/Projects-SHARPy/aeroelasticPMOR_Optimization/design_of_experiments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="8_{ED382843-3369-464F-9552-85627E9C2B68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2AE2FAB9-1739-4C34-95DC-DD0C6FD8E7C8}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="11_99D332F0F8BEEA0CB90F33BCDBB997257A3E9B2E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8977413E-216C-49B1-8A87-CB96E84A8589}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="10110" yWindow="3105" windowWidth="19035" windowHeight="12840" xr2:uid="{85F0F2F6-30EB-4AA0-9047-6E03072A04A5}"/>
+    <workbookView minimized="1" xWindow="2730" yWindow="2730" windowWidth="19035" windowHeight="12840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>Results of criterion</t>
   </si>
@@ -49,6 +40,15 @@
   </si>
   <si>
     <t>Optimisation</t>
+  </si>
+  <si>
+    <t>Comparing Spiral vs Structured using sum(1/d) criteria</t>
+  </si>
+  <si>
+    <t>Spiral</t>
+  </si>
+  <si>
+    <t>Structured</t>
   </si>
 </sst>
 </file>
@@ -56,15 +56,15 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -89,7 +89,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -403,14 +403,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD8EA3A8-1F41-4D0A-A9F7-C5E51732898D}">
-  <dimension ref="A1:D7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -460,7 +460,68 @@
         <v>81.227910109338296</v>
       </c>
     </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>4</v>
+      </c>
+      <c r="B12" s="1">
+        <v>2.6423254318158702</v>
+      </c>
+      <c r="C12" s="1">
+        <v>2.7316634235818902</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>9</v>
+      </c>
+      <c r="B13" s="1">
+        <v>8.8148050166905101</v>
+      </c>
+      <c r="C13" s="1">
+        <v>8.3793569722851799</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>16</v>
+      </c>
+      <c r="B14" s="1">
+        <v>19.1080983555775</v>
+      </c>
+      <c r="C14" s="1">
+        <v>16.971715494995902</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>25</v>
+      </c>
+      <c r="B15" s="1">
+        <v>33.933145084621202</v>
+      </c>
+      <c r="C15" s="1">
+        <v>28.508849662534701</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>